<commit_message>
ajout du reprofilage, du rechapitrage et du périmètre
</commit_message>
<xml_diff>
--- a/convergence-export/src/main/resources/template-export-convergence.xlsx
+++ b/convergence-export/src/main/resources/template-export-convergence.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjuillard\Documents\segur\squash-convergence-export-plugin\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flabatie\Documents\ENV-ANS\19-PLUGIN-SQUASH\Claire2\squash-plugin\convergence-export\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ABB709-7583-4887-8F58-3BE32780270E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2E9D12-3485-44FF-A65A-B775DA7DE925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33360" yWindow="-3480" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14520" yWindow="-18120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exigences" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Exigences!$B$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Exigences!$C$1:$J$1</definedName>
     <definedName name="appDefaut">#REF!</definedName>
     <definedName name="Applicable">#REF!</definedName>
     <definedName name="appNonApp">#REF!</definedName>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Profil</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>Preuve</t>
+  </si>
+  <si>
+    <t>Profil historique</t>
+  </si>
+  <si>
+    <t>Périmètre</t>
+  </si>
+  <si>
+    <t>Vague 1</t>
   </si>
 </sst>
 </file>
@@ -123,39 +132,39 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -227,7 +236,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -262,17 +271,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -297,6 +295,21 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -578,87 +591,101 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil5"/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.25" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.2109375" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="37.9140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="66.4140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.58203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="66.4140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="18.58203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="30.58203125" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="9.25" style="7"/>
+    <col min="1" max="1" width="13.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="13.2109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.92578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.2109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="66.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.2109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="66.42578125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="9.2109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="56.25" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="56.25" customHeight="1">
+      <c r="A1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="19" t="s">
         <v>15</v>
       </c>
+      <c r="K1" s="17" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" s="18" customFormat="1" ht="68.25" customHeight="1">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:11" s="15" customFormat="1" ht="68.25" customHeight="1">
+      <c r="A2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="H2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="I2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="J2" s="20" t="s">
         <v>8</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:I2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="C1:J2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout de la colonne ordre
</commit_message>
<xml_diff>
--- a/convergence-export/src/main/resources/template-export-convergence.xlsx
+++ b/convergence-export/src/main/resources/template-export-convergence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flabatie\Documents\ENV-ANS\19-PLUGIN-SQUASH\Claire2\squash-plugin\convergence-export\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0655D3-A27D-4F9D-8473-FAD1279F3DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DBD490-DDE1-4A0F-99AB-C96067D90A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14520" yWindow="-18120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exigences" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Profil</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Mineure</t>
+  </si>
+  <si>
+    <t>Ordre</t>
   </si>
 </sst>
 </file>
@@ -597,11 +600,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil5"/>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.2109375" defaultRowHeight="15.5"/>
@@ -621,7 +624,7 @@
     <col min="13" max="16384" width="9.2109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="56.25" customHeight="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="56.25" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>17</v>
       </c>
@@ -658,8 +661,11 @@
       <c r="L1" s="17" t="s">
         <v>19</v>
       </c>
+      <c r="M1" s="17" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" s="15" customFormat="1" ht="68.25" customHeight="1">
+    <row r="2" spans="1:13" s="15" customFormat="1" ht="68.25" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
@@ -695,6 +701,9 @@
       </c>
       <c r="L2" s="10" t="s">
         <v>20</v>
+      </c>
+      <c r="M2" s="10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout/deplacement de la colonne commentaire
</commit_message>
<xml_diff>
--- a/convergence-export/src/main/resources/template-export-convergence.xlsx
+++ b/convergence-export/src/main/resources/template-export-convergence.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flabatie\Documents\ENV-ANS\19-PLUGIN-SQUASH\Claire2\squash-plugin\convergence-export\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DBD490-DDE1-4A0F-99AB-C96067D90A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A882C8-E632-4EFB-B7F1-70182D36876E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15675" yWindow="-18120" windowWidth="27645" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exigences" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Exigences!$C$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Exigences!$C$1:$K$1</definedName>
     <definedName name="appDefaut">#REF!</definedName>
     <definedName name="Applicable">#REF!</definedName>
     <definedName name="appNonApp">#REF!</definedName>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Profil</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>Ordre</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -600,11 +606,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil5"/>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.2109375" defaultRowHeight="15.5"/>
@@ -614,17 +620,18 @@
     <col min="3" max="3" width="37.92578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="35.2109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="66.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.2109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="66.42578125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" style="7" customWidth="1"/>
-    <col min="12" max="12" width="12.35546875" style="7" customWidth="1"/>
-    <col min="13" max="16384" width="9.2109375" style="7"/>
+    <col min="6" max="6" width="32.78515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.2109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="66.42578125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="30.5703125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" style="7" customWidth="1"/>
+    <col min="13" max="13" width="12.35546875" style="7" customWidth="1"/>
+    <col min="14" max="16384" width="9.2109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="56.25" customHeight="1">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="56.25" customHeight="1">
       <c r="A1" s="17" t="s">
         <v>17</v>
       </c>
@@ -640,32 +647,35 @@
       <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="K1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="L1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="15" customFormat="1" ht="68.25" customHeight="1">
+    <row r="2" spans="1:14" s="15" customFormat="1" ht="68.25" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
@@ -681,33 +691,36 @@
       <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="K2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="M2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="10">
+      <c r="N2" s="10">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:J2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="C1:K2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>